<commit_message>
Update code and add more config
</commit_message>
<xml_diff>
--- a/Doc/Brivis Protocol.xlsx
+++ b/Doc/Brivis Protocol.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\Brivis Networker\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5C85E1-74ED-40FD-BC43-ED7CC0F855CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F9E47-AE75-4690-B999-45DBBFF3E446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35220" yWindow="5100" windowWidth="21660" windowHeight="22545" xr2:uid="{998ADE95-1D2A-4FF7-8A41-9C1B9895771B}"/>
+    <workbookView xWindow="12660" yWindow="4800" windowWidth="20025" windowHeight="22545" xr2:uid="{998ADE95-1D2A-4FF7-8A41-9C1B9895771B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="122">
   <si>
     <t>Command</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Set temperature in full degrees</t>
   </si>
   <si>
-    <t>Actual temperaure if 1/2 degrees</t>
-  </si>
-  <si>
     <t>The payload contains 6 bytes</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>Current hour (24 hour)</t>
   </si>
   <si>
-    <t>00=Set temp less than actual, FF=Set temp equal or more than actual</t>
-  </si>
-  <si>
     <t>LSB of counter</t>
   </si>
   <si>
@@ -396,6 +390,15 @@
   </si>
   <si>
     <t>Always 00 or 01</t>
+  </si>
+  <si>
+    <t>Calling it SendIdle</t>
+  </si>
+  <si>
+    <t>Actual temperaure in 1/2 degrees</t>
+  </si>
+  <si>
+    <t>00=Current temp is more than set temp, FF=Current temp is less than or equal to set temp</t>
   </si>
 </sst>
 </file>
@@ -816,8 +819,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,10 +925,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,7 +936,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,7 +1026,7 @@
         <v>41</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -1033,7 +1036,7 @@
         <v>42</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -1069,7 +1072,7 @@
         <v>45</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -1178,7 +1181,7 @@
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1211,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1229,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F57" s="6"/>
     </row>
@@ -1248,6 +1251,9 @@
       <c r="C60" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="E60" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
@@ -1350,7 +1356,7 @@
         <v>32</v>
       </c>
       <c r="D75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -1377,7 +1383,7 @@
         <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -1386,7 +1392,7 @@
         <v>3</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -1395,10 +1401,10 @@
         <v>4</v>
       </c>
       <c r="D80" t="s">
+        <v>115</v>
+      </c>
+      <c r="F80" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="G80" s="6"/>
     </row>
@@ -1408,7 +1414,7 @@
         <v>5</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1421,10 +1427,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C84" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,7 +1438,7 @@
         <v>16</v>
       </c>
       <c r="D85" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,7 +1446,7 @@
         <v>19</v>
       </c>
       <c r="D86" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,7 +1462,7 @@
         <v>18</v>
       </c>
       <c r="D88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,7 +1470,7 @@
         <v>7</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,7 +1479,7 @@
       </c>
       <c r="C91" s="11"/>
       <c r="D91" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,7 +1495,7 @@
         <v>32</v>
       </c>
       <c r="D93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1498,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1511,10 +1517,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C97" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,7 +1528,7 @@
         <v>16</v>
       </c>
       <c r="D98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,7 +1544,7 @@
         <v>32</v>
       </c>
       <c r="D100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,7 +1569,7 @@
         <v>8</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,7 +1577,7 @@
         <v>16</v>
       </c>
       <c r="D105" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,7 +1593,7 @@
         <v>32</v>
       </c>
       <c r="D107" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1595,7 +1601,7 @@
         <v>18</v>
       </c>
       <c r="D108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,7 +1617,7 @@
         <v>16</v>
       </c>
       <c r="D111" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,7 +1625,7 @@
         <v>19</v>
       </c>
       <c r="D112" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -1635,301 +1641,301 @@
         <v>18</v>
       </c>
       <c r="D114" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
+        <v>96</v>
+      </c>
+      <c r="E121" t="s">
         <v>97</v>
-      </c>
-      <c r="E121" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
+        <v>82</v>
+      </c>
+      <c r="E122" t="s">
         <v>83</v>
-      </c>
-      <c r="E122" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E123" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
+        <v>82</v>
+      </c>
+      <c r="E124" t="s">
         <v>83</v>
-      </c>
-      <c r="E124" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E125" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
+        <v>82</v>
+      </c>
+      <c r="E126" t="s">
         <v>83</v>
-      </c>
-      <c r="E126" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E127" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
+        <v>82</v>
+      </c>
+      <c r="E128" t="s">
         <v>83</v>
-      </c>
-      <c r="E128" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E129" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
+        <v>82</v>
+      </c>
+      <c r="E130" t="s">
         <v>83</v>
-      </c>
-      <c r="E130" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E131" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
+        <v>82</v>
+      </c>
+      <c r="E132" t="s">
         <v>83</v>
-      </c>
-      <c r="E132" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
+        <v>84</v>
+      </c>
+      <c r="E133" t="s">
         <v>85</v>
-      </c>
-      <c r="E133" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E134" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
+        <v>82</v>
+      </c>
+      <c r="E135" t="s">
         <v>83</v>
-      </c>
-      <c r="E135" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
+        <v>84</v>
+      </c>
+      <c r="E136" t="s">
         <v>85</v>
-      </c>
-      <c r="E136" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E137" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
+        <v>82</v>
+      </c>
+      <c r="E138" t="s">
         <v>83</v>
-      </c>
-      <c r="E138" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E139" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E143" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" t="s">
+        <v>82</v>
+      </c>
+      <c r="E144" t="s">
         <v>83</v>
-      </c>
-      <c r="E144" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" t="s">
+        <v>84</v>
+      </c>
+      <c r="E145" t="s">
         <v>85</v>
-      </c>
-      <c r="E145" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" t="s">
+        <v>82</v>
+      </c>
+      <c r="E146" t="s">
         <v>83</v>
-      </c>
-      <c r="E146" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E147" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" t="s">
+        <v>82</v>
+      </c>
+      <c r="E148" t="s">
         <v>83</v>
-      </c>
-      <c r="E148" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="9"/>
       <c r="B149" t="s">
+        <v>84</v>
+      </c>
+      <c r="E149" t="s">
         <v>85</v>
-      </c>
-      <c r="E149" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="9"/>
       <c r="B150" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E150" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="9"/>
       <c r="B151" t="s">
+        <v>82</v>
+      </c>
+      <c r="E151" t="s">
         <v>83</v>
-      </c>
-      <c r="E151" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="9"/>
       <c r="B152" t="s">
+        <v>84</v>
+      </c>
+      <c r="E152" t="s">
         <v>85</v>
-      </c>
-      <c r="E152" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="9"/>
       <c r="B153" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E153" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="9"/>
       <c r="B154" t="s">
+        <v>82</v>
+      </c>
+      <c r="E154" t="s">
         <v>83</v>
-      </c>
-      <c r="E154" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="9"/>
       <c r="B155" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E155" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,12 +1943,12 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>